<commit_message>
Correcion validacion fecha inventario
</commit_message>
<xml_diff>
--- a/Base clientes.xlsx
+++ b/Base clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad2196898358a5cd/Documentos/SellOut ConAgro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F15C827-0D51-4023-885E-CB6439432888}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3386017-970F-4324-8858-AA38D12C613A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21336" windowHeight="11376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Clientes carga manual" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Num_Distri</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>AGROIMPULSORA CUAMANCO</t>
+  </si>
+  <si>
+    <t>DIABONOS S.A.</t>
+  </si>
+  <si>
+    <t>ARIANNA GARCIA</t>
+  </si>
+  <si>
+    <t>Agroquimicos Libra</t>
+  </si>
+  <si>
+    <t>ASESORIA INTEGRAL LUMINARIAS</t>
   </si>
 </sst>
 </file>
@@ -60,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -117,7 +129,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -150,8 +162,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:B15" totalsRowShown="0">
+  <autoFilter ref="A1:B15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Num_Distri"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name_Distri"/>
@@ -448,10 +460,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,7 +506,7 @@
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>10210128</v>
+        <v>500226</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -538,6 +550,46 @@
       </c>
       <c r="B10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>62000076</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10236216</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>10234501</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>10220649</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>10234501</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega validación de fecha
</commit_message>
<xml_diff>
--- a/Base clientes.xlsx
+++ b/Base clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad2196898358a5cd/Documentos/SellOut ConAgro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3386017-970F-4324-8858-AA38D12C613A}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0999DC-1447-4980-9066-0D14B354D008}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21336" windowHeight="11376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Clientes carga manual" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Num_Distri</t>
   </si>
@@ -65,14 +65,28 @@
   </si>
   <si>
     <t>ASESORIA INTEGRAL LUMINARIAS</t>
+  </si>
+  <si>
+    <t>MARIA GUADALUPE RUIZ ESTRADA</t>
+  </si>
+  <si>
+    <t>AGRICOLA EL MORON SA DE CV</t>
+  </si>
+  <si>
+    <t>INSECTICIDAS HERBICIDAS Y SEMILLAS RIDA</t>
+  </si>
+  <si>
+    <t>DUNE COMPANY MEXICALI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -126,10 +140,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -143,10 +167,20 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
+    <cellStyle name="Millares 2" xfId="7" xr:uid="{BD6E2458-1F3F-42E6-BABE-03930E1447CB}"/>
+    <cellStyle name="Millares 3" xfId="12" xr:uid="{95B82810-E653-4171-BB54-2CD7CC33F282}"/>
     <cellStyle name="Moneda 2" xfId="2" xr:uid="{B9BDF5DC-8F79-4411-B0C0-5063B63F63CE}"/>
+    <cellStyle name="Moneda 2 2" xfId="6" xr:uid="{E93832B5-631C-4752-BFF8-953B07358624}"/>
+    <cellStyle name="Moneda 2 3" xfId="4" xr:uid="{4C27931F-DE21-4C2B-89CC-7DF3B356D943}"/>
+    <cellStyle name="Moneda 3" xfId="9" xr:uid="{082D24A5-AE21-4816-B6DC-97412EFF2A3A}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DBBBE059-1A68-410B-956D-065054F07D32}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{DD442545-9EA6-417D-99C8-52B3BCEBBA20}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{A00F9122-2F87-4D49-8DD1-5BF2D7ED3404}"/>
+    <cellStyle name="Normal 5" xfId="8" xr:uid="{39BE2B1D-27CE-4A5D-A7E4-F42BB133DAF8}"/>
+    <cellStyle name="Normal 6" xfId="10" xr:uid="{9F50ACCD-DF49-4CEE-94A1-AC61E99D16EB}"/>
+    <cellStyle name="Normal 7" xfId="11" xr:uid="{CBEEB419-4C15-4833-9DE5-0864A1697C9B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -162,8 +196,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:B15" totalsRowShown="0">
-  <autoFilter ref="A1:B15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:B19" totalsRowShown="0">
+  <autoFilter ref="A1:B19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Num_Distri"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name_Distri"/>
@@ -460,16 +494,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -590,6 +624,38 @@
       </c>
       <c r="B15" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>10240057</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>10174274</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>500231</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>10181721</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega validación de fecha para Ecuaquimica
</commit_message>
<xml_diff>
--- a/Base clientes.xlsx
+++ b/Base clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad2196898358a5cd/Documentos/SellOut ConAgro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0999DC-1447-4980-9066-0D14B354D008}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E4D1FD-410C-4866-856B-35DB1D295115}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26280" yWindow="1170" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Clientes carga manual" sheetId="1" r:id="rId1"/>
@@ -83,10 +83,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -153,7 +152,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -497,7 +496,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Se agrega la documentación de usuario para el RPA ConAgro
</commit_message>
<xml_diff>
--- a/Base clientes.xlsx
+++ b/Base clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad2196898358a5cd/Documentos/SellOut ConAgro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E4D1FD-410C-4866-856B-35DB1D295115}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81EAE252-F318-49E1-960E-9458142F3329}"/>
   <bookViews>
-    <workbookView xWindow="26280" yWindow="1170" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2745" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Clientes carga manual" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Num_Distri</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>DUNE COMPANY MEXICALI</t>
+  </si>
+  <si>
+    <t>AGROINSUMOS DEL CENTRO</t>
+  </si>
+  <si>
+    <t>MAS AGROQUIMICOS Y SEMILLAS</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -153,6 +159,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -166,7 +174,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Millares 2" xfId="7" xr:uid="{BD6E2458-1F3F-42E6-BABE-03930E1447CB}"/>
     <cellStyle name="Millares 3" xfId="12" xr:uid="{95B82810-E653-4171-BB54-2CD7CC33F282}"/>
     <cellStyle name="Moneda 2" xfId="2" xr:uid="{B9BDF5DC-8F79-4411-B0C0-5063B63F63CE}"/>
@@ -180,6 +188,8 @@
     <cellStyle name="Normal 5" xfId="8" xr:uid="{39BE2B1D-27CE-4A5D-A7E4-F42BB133DAF8}"/>
     <cellStyle name="Normal 6" xfId="10" xr:uid="{9F50ACCD-DF49-4CEE-94A1-AC61E99D16EB}"/>
     <cellStyle name="Normal 7" xfId="11" xr:uid="{CBEEB419-4C15-4833-9DE5-0864A1697C9B}"/>
+    <cellStyle name="Normal 8" xfId="13" xr:uid="{B220FB48-B159-44DE-8DDE-05C3BA6A591C}"/>
+    <cellStyle name="Normal 9" xfId="14" xr:uid="{E35EC62F-D911-4BAE-90D6-5A9FF14CCB46}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -195,8 +205,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:B19" totalsRowShown="0">
-  <autoFilter ref="A1:B19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:B21" totalsRowShown="0">
+  <autoFilter ref="A1:B21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Num_Distri"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name_Distri"/>
@@ -493,19 +503,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>61610097</v>
       </c>
@@ -521,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>61610107</v>
       </c>
@@ -529,7 +539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>10268259</v>
       </c>
@@ -537,7 +547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>500226</v>
       </c>
@@ -545,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>10317368</v>
       </c>
@@ -553,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>500619</v>
       </c>
@@ -561,7 +571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10174274</v>
       </c>
@@ -569,7 +579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>10380667</v>
       </c>
@@ -577,7 +587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10245796</v>
       </c>
@@ -585,7 +595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>62000076</v>
       </c>
@@ -593,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10236216</v>
       </c>
@@ -601,7 +611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10234501</v>
       </c>
@@ -609,7 +619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>10220649</v>
       </c>
@@ -617,7 +627,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>10234501</v>
       </c>
@@ -625,7 +635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>10240057</v>
       </c>
@@ -633,7 +643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>10174274</v>
       </c>
@@ -641,7 +651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>500231</v>
       </c>
@@ -649,12 +659,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>10181721</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>500258</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>10268402</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>